<commit_message>
Minor tweeks to autopilot and OCA classes.
</commit_message>
<xml_diff>
--- a/UAV_Waypoints.xlsx
+++ b/UAV_Waypoints.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="14355" windowHeight="5190" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="195" windowWidth="14355" windowHeight="5130" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -308,11 +308,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="118490624"/>
-        <c:axId val="118492160"/>
+        <c:axId val="126115200"/>
+        <c:axId val="126145664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="118490624"/>
+        <c:axId val="126115200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -346,14 +346,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118492160"/>
+        <c:crossAx val="126145664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
         <c:minorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="118492160"/>
+        <c:axId val="126145664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4.5"/>
@@ -387,7 +387,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118490624"/>
+        <c:crossAx val="126115200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
@@ -532,11 +532,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="118520832"/>
-        <c:axId val="118530816"/>
+        <c:axId val="134430080"/>
+        <c:axId val="134476928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="118520832"/>
+        <c:axId val="134430080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -570,14 +570,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118530816"/>
+        <c:crossAx val="134476928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
         <c:minorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="118530816"/>
+        <c:axId val="134476928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4.5"/>
@@ -611,7 +611,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118520832"/>
+        <c:crossAx val="134430080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
@@ -756,11 +756,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="121721216"/>
-        <c:axId val="121722752"/>
+        <c:axId val="118563968"/>
+        <c:axId val="118565504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121721216"/>
+        <c:axId val="118563968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -794,14 +794,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121722752"/>
+        <c:crossAx val="118565504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
         <c:minorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121722752"/>
+        <c:axId val="118565504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4.5"/>
@@ -835,7 +835,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121721216"/>
+        <c:crossAx val="118563968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
@@ -980,11 +980,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="121751040"/>
-        <c:axId val="121752576"/>
+        <c:axId val="124823808"/>
+        <c:axId val="127877120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121751040"/>
+        <c:axId val="124823808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1018,14 +1018,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121752576"/>
+        <c:crossAx val="127877120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
         <c:minorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121752576"/>
+        <c:axId val="127877120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4.5"/>
@@ -1059,7 +1059,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121751040"/>
+        <c:crossAx val="124823808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
@@ -3481,7 +3481,7 @@
   <dimension ref="A1:G262"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3531,10 +3531,10 @@
         <v>13</v>
       </c>
       <c r="C8" s="14">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="D8" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F8" s="9">
         <v>15000</v>
@@ -3591,23 +3591,23 @@
       </c>
       <c r="C12" s="12">
         <f ca="1">(($C$9*RAND()*2)-$C$9)+$C$8</f>
-        <v>-1.6727091772306972</v>
+        <v>-0.29949781048265578</v>
       </c>
       <c r="D12" s="12">
         <f ca="1">(($D$9*RAND()*2)-$D$9)+$D$8</f>
-        <v>1.406356884315459</v>
+        <v>0.39730728227082945</v>
       </c>
       <c r="E12" s="5">
         <f ca="1">RANDBETWEEN(0,359)</f>
-        <v>131</v>
+        <v>282</v>
       </c>
       <c r="F12" s="11">
         <f t="shared" ref="F12:F36" ca="1" si="0">(($F$9*RAND()*2)-$F$9)+$F$8</f>
-        <v>15189.019328625694</v>
+        <v>14374.046465422336</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" ref="G12:G36" ca="1" si="1">CONCATENATE("UAV_S", TEXT(A12, "00"), $A$1, B12, $A$2, TEXT(F12, "0.0"), $A$3, E12, $A$4, TEXT(C12, "0.000000"), $A$5, TEXT(D12, "0.000000"), $A$6)</f>
-        <v>UAV_S01: ( UAV id: 14 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 15189.0 ) initHeading: ( Degrees 131 ) initXPos: ( NauticalMiles -1.672709 ) initYPos: ( NauticalMiles 1.406357 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
+        <v>UAV_S01: ( UAV id: 14 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 14374.0 ) initHeading: ( Degrees 282 ) initXPos: ( NauticalMiles -0.299498 ) initYPos: ( NauticalMiles 0.397307 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -3621,23 +3621,23 @@
       </c>
       <c r="C13" s="12">
         <f t="shared" ref="C13:C36" ca="1" si="4">(($C$9*RAND()*2)-$C$9)+$C$8</f>
-        <v>-2.4849156531645278</v>
+        <v>-0.59706353079500318</v>
       </c>
       <c r="D13" s="12">
         <f t="shared" ref="D13:D36" ca="1" si="5">(($D$9*RAND()*2)-$D$9)+$D$8</f>
-        <v>1.7848399816639691</v>
+        <v>0.26407083396439668</v>
       </c>
       <c r="E13" s="5">
         <f t="shared" ref="E13:E36" ca="1" si="6">RANDBETWEEN(0,359)</f>
-        <v>306</v>
+        <v>93</v>
       </c>
       <c r="F13" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>15282.633979967206</v>
+        <v>14610.684456966734</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UAV_S02: ( UAV id: 15 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 15282.6 ) initHeading: ( Degrees 306 ) initXPos: ( NauticalMiles -2.484916 ) initYPos: ( NauticalMiles 1.784840 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
+        <v>UAV_S02: ( UAV id: 15 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 14610.7 ) initHeading: ( Degrees 93 ) initXPos: ( NauticalMiles -0.597064 ) initYPos: ( NauticalMiles 0.264071 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -3651,23 +3651,23 @@
       </c>
       <c r="C14" s="12">
         <f t="shared" ca="1" si="4"/>
-        <v>-2.2200002669330301</v>
+        <v>3.5843470604429051E-2</v>
       </c>
       <c r="D14" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>1.0381276094835883</v>
+        <v>2.2246344746519764E-2</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>59</v>
+        <v>262</v>
       </c>
       <c r="F14" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>16386.008890660676</v>
+        <v>13292.885213346492</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UAV_S03: ( UAV id: 16 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 16386.0 ) initHeading: ( Degrees 59 ) initXPos: ( NauticalMiles -2.220000 ) initYPos: ( NauticalMiles 1.038128 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
+        <v>UAV_S03: ( UAV id: 16 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 13292.9 ) initHeading: ( Degrees 262 ) initXPos: ( NauticalMiles 0.035843 ) initYPos: ( NauticalMiles 0.022246 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -3681,23 +3681,23 @@
       </c>
       <c r="C15" s="12">
         <f t="shared" ca="1" si="4"/>
-        <v>-1.7634926224375749</v>
+        <v>0.48087368203200631</v>
       </c>
       <c r="D15" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>1.3918927092841746</v>
+        <v>-0.37819063599684455</v>
       </c>
       <c r="E15" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>45</v>
+        <v>218</v>
       </c>
       <c r="F15" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>16750.815495056573</v>
+        <v>14193.592874645496</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UAV_S04: ( UAV id: 17 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 16750.8 ) initHeading: ( Degrees 45 ) initXPos: ( NauticalMiles -1.763493 ) initYPos: ( NauticalMiles 1.391893 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
+        <v>UAV_S04: ( UAV id: 17 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 14193.6 ) initHeading: ( Degrees 218 ) initXPos: ( NauticalMiles 0.480874 ) initYPos: ( NauticalMiles -0.378191 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -3711,23 +3711,23 @@
       </c>
       <c r="C16" s="12">
         <f t="shared" ca="1" si="4"/>
-        <v>-2.5543427371967873</v>
+        <v>0.51213046523304206</v>
       </c>
       <c r="D16" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>1.1447956825940293</v>
+        <v>-0.65476611276087859</v>
       </c>
       <c r="E16" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>206</v>
+        <v>20</v>
       </c>
       <c r="F16" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>14299.049787667471</v>
+        <v>13630.893573489237</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UAV_S05: ( UAV id: 18 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 14299.0 ) initHeading: ( Degrees 206 ) initXPos: ( NauticalMiles -2.554343 ) initYPos: ( NauticalMiles 1.144796 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
+        <v>UAV_S05: ( UAV id: 18 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 13630.9 ) initHeading: ( Degrees 20 ) initXPos: ( NauticalMiles 0.512130 ) initYPos: ( NauticalMiles -0.654766 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -3741,23 +3741,23 @@
       </c>
       <c r="C17" s="12">
         <f t="shared" ca="1" si="4"/>
-        <v>-1.4554751655062528</v>
+        <v>-0.14897755687905723</v>
       </c>
       <c r="D17" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>1.0228259477712827</v>
+        <v>-0.14828751073067892</v>
       </c>
       <c r="E17" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>344</v>
+        <v>285</v>
       </c>
       <c r="F17" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>13966.690928224196</v>
+        <v>16432.518160691197</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UAV_S06: ( UAV id: 19 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 13966.7 ) initHeading: ( Degrees 344 ) initXPos: ( NauticalMiles -1.455475 ) initYPos: ( NauticalMiles 1.022826 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
+        <v>UAV_S06: ( UAV id: 19 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 16432.5 ) initHeading: ( Degrees 285 ) initXPos: ( NauticalMiles -0.148978 ) initYPos: ( NauticalMiles -0.148288 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -3771,23 +3771,23 @@
       </c>
       <c r="C18" s="12">
         <f t="shared" ca="1" si="4"/>
-        <v>-1.440403065300577</v>
+        <v>-0.80906444173644654</v>
       </c>
       <c r="D18" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>2.1475970955273853</v>
+        <v>0.86298101450109255</v>
       </c>
       <c r="E18" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>229</v>
+        <v>116</v>
       </c>
       <c r="F18" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>15187.450561275364</v>
+        <v>13243.322771478825</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UAV_S07: ( UAV id: 20 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 15187.5 ) initHeading: ( Degrees 229 ) initXPos: ( NauticalMiles -1.440403 ) initYPos: ( NauticalMiles 2.147597 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
+        <v>UAV_S07: ( UAV id: 20 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 13243.3 ) initHeading: ( Degrees 116 ) initXPos: ( NauticalMiles -0.809064 ) initYPos: ( NauticalMiles 0.862981 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -3801,23 +3801,23 @@
       </c>
       <c r="C19" s="12">
         <f t="shared" ca="1" si="4"/>
-        <v>-1.8231385049713966</v>
+        <v>-0.7544948778128111</v>
       </c>
       <c r="D19" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>2.7341117906576144</v>
+        <v>0.8992597615430038</v>
       </c>
       <c r="E19" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>229</v>
+        <v>7</v>
       </c>
       <c r="F19" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>13848.242390073037</v>
+        <v>14737.644028548206</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UAV_S08: ( UAV id: 21 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 13848.2 ) initHeading: ( Degrees 229 ) initXPos: ( NauticalMiles -1.823139 ) initYPos: ( NauticalMiles 2.734112 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
+        <v>UAV_S08: ( UAV id: 21 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 14737.6 ) initHeading: ( Degrees 7 ) initXPos: ( NauticalMiles -0.754495 ) initYPos: ( NauticalMiles 0.899260 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -3831,23 +3831,23 @@
       </c>
       <c r="C20" s="12">
         <f t="shared" ca="1" si="4"/>
-        <v>-2.0375538559877278</v>
+        <v>0.53546370494941709</v>
       </c>
       <c r="D20" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>1.6617269110328987</v>
+        <v>-0.20100301295630119</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>335</v>
+        <v>140</v>
       </c>
       <c r="F20" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>14699.239778371088</v>
+        <v>16369.015998572966</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UAV_S09: ( UAV id: 22 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 14699.2 ) initHeading: ( Degrees 335 ) initXPos: ( NauticalMiles -2.037554 ) initYPos: ( NauticalMiles 1.661727 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
+        <v>UAV_S09: ( UAV id: 22 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 16369.0 ) initHeading: ( Degrees 140 ) initXPos: ( NauticalMiles 0.535464 ) initYPos: ( NauticalMiles -0.201003 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -3861,23 +3861,23 @@
       </c>
       <c r="C21" s="12">
         <f t="shared" ca="1" si="4"/>
-        <v>-1.2501503091731843</v>
+        <v>0.12470825259255691</v>
       </c>
       <c r="D21" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>2.1873797404425837</v>
+        <v>-0.45732136342552443</v>
       </c>
       <c r="E21" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>252</v>
+        <v>291</v>
       </c>
       <c r="F21" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>14318.778140318569</v>
+        <v>16590.003006522133</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UAV_S10: ( UAV id: 23 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 14318.8 ) initHeading: ( Degrees 252 ) initXPos: ( NauticalMiles -1.250150 ) initYPos: ( NauticalMiles 2.187380 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
+        <v>UAV_S10: ( UAV id: 23 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 16590.0 ) initHeading: ( Degrees 291 ) initXPos: ( NauticalMiles 0.124708 ) initYPos: ( NauticalMiles -0.457321 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -3891,23 +3891,23 @@
       </c>
       <c r="C22" s="12">
         <f t="shared" ca="1" si="4"/>
-        <v>-2.5877286132045874</v>
+        <v>-0.10645101031754534</v>
       </c>
       <c r="D22" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>2.7589205995332309</v>
+        <v>0.78455064666738705</v>
       </c>
       <c r="E22" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>236</v>
+        <v>139</v>
       </c>
       <c r="F22" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>13238.960617542674</v>
+        <v>14702.673599736139</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UAV_S11: ( UAV id: 24 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 13239.0 ) initHeading: ( Degrees 236 ) initXPos: ( NauticalMiles -2.587729 ) initYPos: ( NauticalMiles 2.758921 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
+        <v>UAV_S11: ( UAV id: 24 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 14702.7 ) initHeading: ( Degrees 139 ) initXPos: ( NauticalMiles -0.106451 ) initYPos: ( NauticalMiles 0.784551 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -3921,23 +3921,23 @@
       </c>
       <c r="C23" s="12">
         <f t="shared" ca="1" si="4"/>
-        <v>-2.5017656021954586</v>
+        <v>0.15237843218172653</v>
       </c>
       <c r="D23" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>1.9658536922654932</v>
+        <v>-0.20241655528029412</v>
       </c>
       <c r="E23" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>19</v>
+        <v>107</v>
       </c>
       <c r="F23" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>14385.077327868576</v>
+        <v>13606.7345177733</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UAV_S12: ( UAV id: 25 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 14385.1 ) initHeading: ( Degrees 19 ) initXPos: ( NauticalMiles -2.501766 ) initYPos: ( NauticalMiles 1.965854 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
+        <v>UAV_S12: ( UAV id: 25 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 13606.7 ) initHeading: ( Degrees 107 ) initXPos: ( NauticalMiles 0.152378 ) initYPos: ( NauticalMiles -0.202417 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -3951,23 +3951,23 @@
       </c>
       <c r="C24" s="12">
         <f t="shared" ca="1" si="4"/>
-        <v>-2.2130156412435062</v>
+        <v>-0.78195532491022335</v>
       </c>
       <c r="D24" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>2.7837109469000385</v>
+        <v>0.9270626446644108</v>
       </c>
       <c r="E24" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>98</v>
+        <v>271</v>
       </c>
       <c r="F24" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>13777.35661251923</v>
+        <v>14862.741565832555</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UAV_S13: ( UAV id: 26 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 13777.4 ) initHeading: ( Degrees 98 ) initXPos: ( NauticalMiles -2.213016 ) initYPos: ( NauticalMiles 2.783711 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
+        <v>UAV_S13: ( UAV id: 26 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 14862.7 ) initHeading: ( Degrees 271 ) initXPos: ( NauticalMiles -0.781955 ) initYPos: ( NauticalMiles 0.927063 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -3981,23 +3981,23 @@
       </c>
       <c r="C25" s="12">
         <f t="shared" ca="1" si="4"/>
-        <v>-1.8220451787102303</v>
+        <v>-7.6248793245816682E-3</v>
       </c>
       <c r="D25" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>1.8052424586484508</v>
+        <v>0.8774011398212207</v>
       </c>
       <c r="E25" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>338</v>
+        <v>140</v>
       </c>
       <c r="F25" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>15531.321409106771</v>
+        <v>16934.719268147197</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UAV_S14: ( UAV id: 27 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 15531.3 ) initHeading: ( Degrees 338 ) initXPos: ( NauticalMiles -1.822045 ) initYPos: ( NauticalMiles 1.805242 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
+        <v>UAV_S14: ( UAV id: 27 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 16934.7 ) initHeading: ( Degrees 140 ) initXPos: ( NauticalMiles -0.007625 ) initYPos: ( NauticalMiles 0.877401 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -4011,23 +4011,23 @@
       </c>
       <c r="C26" s="12">
         <f t="shared" ca="1" si="4"/>
-        <v>-1.7382016159292422</v>
+        <v>-0.9689214398369923</v>
       </c>
       <c r="D26" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>2.1351553010524107</v>
+        <v>-0.99268286156148244</v>
       </c>
       <c r="E26" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>348</v>
+        <v>92</v>
       </c>
       <c r="F26" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>14293.57057211143</v>
+        <v>14263.74117235389</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UAV_S15: ( UAV id: 28 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 14293.6 ) initHeading: ( Degrees 348 ) initXPos: ( NauticalMiles -1.738202 ) initYPos: ( NauticalMiles 2.135155 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
+        <v>UAV_S15: ( UAV id: 28 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 14263.7 ) initHeading: ( Degrees 92 ) initXPos: ( NauticalMiles -0.968921 ) initYPos: ( NauticalMiles -0.992683 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -4041,23 +4041,23 @@
       </c>
       <c r="C27" s="12">
         <f t="shared" ca="1" si="4"/>
-        <v>-2.9618276326285948</v>
+        <v>-0.86875922989460874</v>
       </c>
       <c r="D27" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>1.0452891109900211</v>
+        <v>0.86423575010867326</v>
       </c>
       <c r="E27" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>331</v>
+        <v>291</v>
       </c>
       <c r="F27" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>13575.54631411954</v>
+        <v>14831.77892827677</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UAV_S16: ( UAV id: 29 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 13575.5 ) initHeading: ( Degrees 331 ) initXPos: ( NauticalMiles -2.961828 ) initYPos: ( NauticalMiles 1.045289 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
+        <v>UAV_S16: ( UAV id: 29 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 14831.8 ) initHeading: ( Degrees 291 ) initXPos: ( NauticalMiles -0.868759 ) initYPos: ( NauticalMiles 0.864236 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -4071,23 +4071,23 @@
       </c>
       <c r="C28" s="12">
         <f t="shared" ca="1" si="4"/>
-        <v>-1.3722704313984553</v>
+        <v>-0.73691191590194927</v>
       </c>
       <c r="D28" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>1.9513741116106949</v>
+        <v>0.95444384289813167</v>
       </c>
       <c r="E28" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>21</v>
+        <v>232</v>
       </c>
       <c r="F28" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>16209.229595161012</v>
+        <v>16447.813577303572</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UAV_S17: ( UAV id: 30 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 16209.2 ) initHeading: ( Degrees 21 ) initXPos: ( NauticalMiles -1.372270 ) initYPos: ( NauticalMiles 1.951374 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
+        <v>UAV_S17: ( UAV id: 30 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 16447.8 ) initHeading: ( Degrees 232 ) initXPos: ( NauticalMiles -0.736912 ) initYPos: ( NauticalMiles 0.954444 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -4101,23 +4101,23 @@
       </c>
       <c r="C29" s="12">
         <f t="shared" ca="1" si="4"/>
-        <v>-2.8486127452437788</v>
+        <v>0.7258956025038763</v>
       </c>
       <c r="D29" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>1.2066430522257059</v>
+        <v>0.28442433391674071</v>
       </c>
       <c r="E29" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>108</v>
+        <v>311</v>
       </c>
       <c r="F29" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>14571.644804686857</v>
+        <v>13241.724377945653</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UAV_S18: ( UAV id: 31 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 14571.6 ) initHeading: ( Degrees 108 ) initXPos: ( NauticalMiles -2.848613 ) initYPos: ( NauticalMiles 1.206643 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
+        <v>UAV_S18: ( UAV id: 31 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 13241.7 ) initHeading: ( Degrees 311 ) initXPos: ( NauticalMiles 0.725896 ) initYPos: ( NauticalMiles 0.284424 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -4131,23 +4131,23 @@
       </c>
       <c r="C30" s="12">
         <f t="shared" ca="1" si="4"/>
-        <v>-1.1860485680768453</v>
+        <v>-0.33047176643024767</v>
       </c>
       <c r="D30" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>2.3438252313010763</v>
+        <v>-0.24019108447886461</v>
       </c>
       <c r="E30" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>116</v>
+        <v>3</v>
       </c>
       <c r="F30" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>14474.338005911937</v>
+        <v>14003.266185837771</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UAV_S19: ( UAV id: 32 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 14474.3 ) initHeading: ( Degrees 116 ) initXPos: ( NauticalMiles -1.186049 ) initYPos: ( NauticalMiles 2.343825 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
+        <v>UAV_S19: ( UAV id: 32 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 14003.3 ) initHeading: ( Degrees 3 ) initXPos: ( NauticalMiles -0.330472 ) initYPos: ( NauticalMiles -0.240191 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -4161,23 +4161,23 @@
       </c>
       <c r="C31" s="12">
         <f t="shared" ca="1" si="4"/>
-        <v>-1.6623836780829826</v>
+        <v>-0.82173012567508774</v>
       </c>
       <c r="D31" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>1.6099421447189803</v>
+        <v>0.17048917700212485</v>
       </c>
       <c r="E31" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>66</v>
+        <v>282</v>
       </c>
       <c r="F31" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>13340.293156591277</v>
+        <v>14557.5515748868</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UAV_S20: ( UAV id: 33 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 13340.3 ) initHeading: ( Degrees 66 ) initXPos: ( NauticalMiles -1.662384 ) initYPos: ( NauticalMiles 1.609942 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
+        <v>UAV_S20: ( UAV id: 33 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 14557.6 ) initHeading: ( Degrees 282 ) initXPos: ( NauticalMiles -0.821730 ) initYPos: ( NauticalMiles 0.170489 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -4191,23 +4191,23 @@
       </c>
       <c r="C32" s="12">
         <f t="shared" ca="1" si="4"/>
-        <v>-1.0184764333094711</v>
+        <v>-0.9674678985252585</v>
       </c>
       <c r="D32" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>2.893352839684221</v>
+        <v>-0.43693797093361231</v>
       </c>
       <c r="E32" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>266</v>
+        <v>190</v>
       </c>
       <c r="F32" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>16383.142538869994</v>
+        <v>16521.285837638155</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UAV_S21: ( UAV id: 34 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 16383.1 ) initHeading: ( Degrees 266 ) initXPos: ( NauticalMiles -1.018476 ) initYPos: ( NauticalMiles 2.893353 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
+        <v>UAV_S21: ( UAV id: 34 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 16521.3 ) initHeading: ( Degrees 190 ) initXPos: ( NauticalMiles -0.967468 ) initYPos: ( NauticalMiles -0.436938 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -4221,23 +4221,23 @@
       </c>
       <c r="C33" s="12">
         <f t="shared" ca="1" si="4"/>
-        <v>-2.0925661483866387</v>
+        <v>0.30871832261787779</v>
       </c>
       <c r="D33" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>2.808598976087473</v>
+        <v>-0.52025636688990073</v>
       </c>
       <c r="E33" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="F33" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>16320.023382951749</v>
+        <v>16712.678132566631</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UAV_S22: ( UAV id: 35 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 16320.0 ) initHeading: ( Degrees 126 ) initXPos: ( NauticalMiles -2.092566 ) initYPos: ( NauticalMiles 2.808599 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
+        <v>UAV_S22: ( UAV id: 35 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 16712.7 ) initHeading: ( Degrees 92 ) initXPos: ( NauticalMiles 0.308718 ) initYPos: ( NauticalMiles -0.520256 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -4251,23 +4251,23 @@
       </c>
       <c r="C34" s="12">
         <f t="shared" ca="1" si="4"/>
-        <v>-2.8851404928179534</v>
+        <v>0.91626722713941433</v>
       </c>
       <c r="D34" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>2.6302124658466677</v>
+        <v>0.91143795859065202</v>
       </c>
       <c r="E34" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F34" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>16768.441951280885</v>
+        <v>14902.08536740493</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UAV_S23: ( UAV id: 36 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 16768.4 ) initHeading: ( Degrees 57 ) initXPos: ( NauticalMiles -2.885140 ) initYPos: ( NauticalMiles 2.630212 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
+        <v>UAV_S23: ( UAV id: 36 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 14902.1 ) initHeading: ( Degrees 70 ) initXPos: ( NauticalMiles 0.916267 ) initYPos: ( NauticalMiles 0.911438 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -4281,23 +4281,23 @@
       </c>
       <c r="C35" s="12">
         <f t="shared" ca="1" si="4"/>
-        <v>-2.9208988695796108</v>
+        <v>0.15016224068289286</v>
       </c>
       <c r="D35" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>1.2817942016354755</v>
+        <v>0.92162578715694798</v>
       </c>
       <c r="E35" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>92</v>
+        <v>153</v>
       </c>
       <c r="F35" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>13351.431757147209</v>
+        <v>15211.489379190501</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UAV_S24: ( UAV id: 37 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 13351.4 ) initHeading: ( Degrees 92 ) initXPos: ( NauticalMiles -2.920899 ) initYPos: ( NauticalMiles 1.281794 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
+        <v>UAV_S24: ( UAV id: 37 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 15211.5 ) initHeading: ( Degrees 153 ) initXPos: ( NauticalMiles 0.150162 ) initYPos: ( NauticalMiles 0.921626 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -4311,23 +4311,23 @@
       </c>
       <c r="C36" s="12">
         <f t="shared" ca="1" si="4"/>
-        <v>-1.4255168021726297</v>
+        <v>-0.19272382953817457</v>
       </c>
       <c r="D36" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>1.4133034798002946</v>
+        <v>0.85916073240289825</v>
       </c>
       <c r="E36" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>247</v>
+        <v>104</v>
       </c>
       <c r="F36" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>13455.071044756764</v>
+        <v>13950.131138722823</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>UAV_S25: ( UAV id: 38 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 13455.1 ) initHeading: ( Degrees 247 ) initXPos: ( NauticalMiles -1.425517 ) initYPos: ( NauticalMiles 1.413303 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
+        <v>UAV_S25: ( UAV id: 38 type: "F-16" initVelocity: 41 side: blue initAlt: ( Feet 13950.1 ) initHeading: ( Degrees 104 ) initXPos: ( NauticalMiles -0.192724 ) initYPos: ( NauticalMiles 0.859161 ) components: { dynamicsModel: ( JSBSimModel rootDir: "../shared/data/JSBSim/" model: "Rascal" ) pilot: ( SimAP mode: "swarm" ) oca: ( OnboardControlAgent desiredSeparation: 2000 ) } )</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>